<commit_message>
LevelUI und Level verändert
</commit_message>
<xml_diff>
--- a/ProjectFiles/Projektmanagement/Arbeitspakete.xlsx
+++ b/ProjectFiles/Projektmanagement/Arbeitspakete.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr showObjects="none" filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EF3AEC-5F65-47B1-82F2-05D94C62EBAC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6B932C-E48D-4F0F-AFC9-8C40D8F77E87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="99">
   <si>
     <t>Nr</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>Animationen, Player-animation</t>
+  </si>
+  <si>
+    <t>Jannis,Selin</t>
   </si>
 </sst>
 </file>
@@ -644,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,6 +1192,9 @@
       <c r="E36" t="s">
         <v>27</v>
       </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
       <c r="G36">
         <v>1</v>
       </c>
@@ -1206,6 +1212,9 @@
       <c r="E37" t="s">
         <v>27</v>
       </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
       <c r="G37">
         <v>1</v>
       </c>
@@ -1286,7 +1295,10 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>27</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
       </c>
       <c r="G42">
         <v>2</v>
@@ -1320,7 +1332,7 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G44">
         <v>2</v>
@@ -1355,6 +1367,9 @@
       </c>
       <c r="E46" t="s">
         <v>91</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1683,7 +1698,7 @@
       </c>
       <c r="F75">
         <f>SUM(F2:F74)</f>
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AP Tabelle updated, Statusbericht von heute
</commit_message>
<xml_diff>
--- a/ProjectFiles/Projektmanagement/Arbeitspakete.xlsx
+++ b/ProjectFiles/Projektmanagement/Arbeitspakete.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr showObjects="none" filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1FBE7F-1AF0-4A2C-8FE9-EBDC98CB7BA8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E4ACB3-10A5-4B1B-A833-F27631761B10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
   <si>
     <t>Nr</t>
   </si>
@@ -348,6 +348,18 @@
   </si>
   <si>
     <t>Stand</t>
+  </si>
+  <si>
+    <t>Code mergen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Rätsel implementiern</t>
+  </si>
+  <si>
+    <t>Rästel ausdenken/beschaffen</t>
   </si>
 </sst>
 </file>
@@ -363,7 +375,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +385,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,13 +428,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -691,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R79"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +730,7 @@
     <col min="4" max="4" width="8.77734375" customWidth="1"/>
     <col min="5" max="5" width="14.21875" customWidth="1"/>
     <col min="6" max="7" width="5.5546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="4.5546875" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" customWidth="1"/>
     <col min="11" max="11" width="5.88671875" customWidth="1"/>
@@ -731,7 +757,7 @@
       <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J1" s="3">
@@ -774,7 +800,7 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>1</v>
       </c>
       <c r="J3" s="3">
@@ -802,7 +828,7 @@
       <c r="F4">
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="J4" s="3">
@@ -830,7 +856,7 @@
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>1</v>
       </c>
       <c r="J5" s="3">
@@ -858,7 +884,7 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>1</v>
       </c>
       <c r="J6" s="3">
@@ -883,7 +909,7 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>1</v>
       </c>
       <c r="J7" s="3">
@@ -905,7 +931,10 @@
       <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="H8">
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="5">
         <v>1</v>
       </c>
       <c r="J8" s="3">
@@ -934,7 +963,7 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>1</v>
       </c>
       <c r="J11" s="3">
@@ -999,7 +1028,7 @@
       <c r="F14">
         <v>5</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>1</v>
       </c>
       <c r="J14" s="3">
@@ -1036,7 +1065,7 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>3</v>
       </c>
       <c r="J15" s="3"/>
@@ -1073,7 +1102,7 @@
       <c r="F16">
         <v>4</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>1</v>
       </c>
       <c r="J16" s="3">
@@ -1110,7 +1139,7 @@
       <c r="F17">
         <v>4</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>1</v>
       </c>
       <c r="J17" s="3">
@@ -1138,7 +1167,7 @@
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>3</v>
       </c>
       <c r="J18" s="3"/>
@@ -1149,16 +1178,36 @@
       <c r="N18" t="s">
         <v>75</v>
       </c>
+      <c r="O18">
+        <v>20</v>
+      </c>
       <c r="P18">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>206</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5">
+        <v>2</v>
+      </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="K19" s="3">
+        <v>5</v>
+      </c>
       <c r="L19" s="3"/>
       <c r="N19" t="s">
         <v>76</v>
+      </c>
+      <c r="O19">
+        <v>20</v>
       </c>
       <c r="P19">
         <v>20</v>
@@ -1171,6 +1220,9 @@
       <c r="N20" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="O20">
+        <v>20</v>
+      </c>
       <c r="P20">
         <v>20</v>
       </c>
@@ -1195,7 +1247,7 @@
       </c>
       <c r="O22">
         <f>SUM(O13:O21)</f>
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="P22">
         <f>SUM(P13:P21)</f>
@@ -1203,7 +1255,7 @@
       </c>
       <c r="Q22">
         <f>SUM(O22:P22)</f>
-        <v>230</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -1225,7 +1277,7 @@
       <c r="F23">
         <v>25</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>1</v>
       </c>
       <c r="J23" s="3">
@@ -1234,7 +1286,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>302</v>
       </c>
@@ -1253,7 +1305,7 @@
       <c r="F24">
         <v>20</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="5">
         <v>1</v>
       </c>
       <c r="J24" s="3">
@@ -1281,7 +1333,7 @@
       <c r="F25">
         <v>1</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>1</v>
       </c>
       <c r="J25" s="3">
@@ -1306,7 +1358,7 @@
       <c r="F26">
         <v>2</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <v>1</v>
       </c>
       <c r="J26" s="3">
@@ -1331,7 +1383,7 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="5">
         <v>1</v>
       </c>
       <c r="J27" s="3">
@@ -1377,7 +1429,7 @@
       <c r="E31" t="s">
         <v>25</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="5">
         <v>2</v>
       </c>
       <c r="J31" s="3"/>
@@ -1434,7 +1486,7 @@
       <c r="F36">
         <v>4</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="5">
         <v>1</v>
       </c>
       <c r="J36" s="3">
@@ -1459,7 +1511,7 @@
       <c r="F37">
         <v>1</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <v>1</v>
       </c>
       <c r="J37" s="3">
@@ -1481,7 +1533,10 @@
       <c r="E38" t="s">
         <v>91</v>
       </c>
-      <c r="H38">
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="H38" s="5">
         <v>1</v>
       </c>
       <c r="J38" s="3">
@@ -1503,7 +1558,7 @@
       <c r="E39" t="s">
         <v>26</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <v>1</v>
       </c>
       <c r="J39" s="3">
@@ -1528,7 +1583,7 @@
       <c r="F40">
         <v>4</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="5">
         <v>2</v>
       </c>
       <c r="J40" s="3"/>
@@ -1547,7 +1602,7 @@
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="5">
         <v>3</v>
       </c>
       <c r="J41" s="3"/>
@@ -1572,7 +1627,7 @@
       <c r="F42">
         <v>2</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="5">
         <v>2</v>
       </c>
       <c r="J42" s="3"/>
@@ -1594,7 +1649,7 @@
       <c r="E43" t="s">
         <v>26</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="5">
         <v>1</v>
       </c>
       <c r="J43" s="3">
@@ -1616,7 +1671,10 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
-      <c r="H44">
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="5">
         <v>2</v>
       </c>
       <c r="J44" s="3"/>
@@ -1638,14 +1696,14 @@
       <c r="E45" t="s">
         <v>25</v>
       </c>
-      <c r="H45">
-        <v>3</v>
+      <c r="H45" s="5">
+        <v>2</v>
       </c>
       <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3">
-        <v>4</v>
-      </c>
+      <c r="K45" s="3">
+        <v>4</v>
+      </c>
+      <c r="L45" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -1663,7 +1721,7 @@
       <c r="F46">
         <v>2</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="5">
         <v>1</v>
       </c>
       <c r="J46" s="3">
@@ -1685,7 +1743,7 @@
       <c r="E47" t="s">
         <v>91</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="5">
         <v>2</v>
       </c>
       <c r="J47" s="3"/>
@@ -1707,7 +1765,7 @@
       <c r="E48" t="s">
         <v>91</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="5">
         <v>2</v>
       </c>
       <c r="J48" s="3"/>
@@ -1732,7 +1790,7 @@
       <c r="F49">
         <v>1</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="5">
         <v>2</v>
       </c>
       <c r="J49" s="3"/>
@@ -1754,7 +1812,7 @@
       <c r="E50" t="s">
         <v>27</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="5">
         <v>3</v>
       </c>
       <c r="J50" s="3"/>
@@ -1764,13 +1822,41 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J51" s="3"/>
+      <c r="A51">
+        <v>517</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>4</v>
+      </c>
+      <c r="J51" s="3">
+        <v>4</v>
+      </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>518</v>
+      </c>
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+      <c r="H52" s="5">
+        <v>2</v>
+      </c>
       <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="K52" s="3">
+        <v>4</v>
+      </c>
       <c r="L52" s="3"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -1779,9 +1865,6 @@
       <c r="L53" s="3"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>49</v>
-      </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -1792,215 +1875,172 @@
       <c r="L55" s="3"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>600</v>
-      </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>601</v>
-      </c>
-      <c r="B57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-      <c r="H57">
-        <v>3</v>
-      </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="3">
-        <v>2</v>
-      </c>
+      <c r="L57" s="3"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58">
-        <v>2</v>
-      </c>
-      <c r="H58">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="3">
-        <v>2</v>
-      </c>
+      <c r="L58" s="3"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="D59">
-        <v>4</v>
-      </c>
-      <c r="E59" t="s">
-        <v>95</v>
-      </c>
-      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="H59" s="5">
         <v>3</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>602</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="H60" s="5">
+        <v>3</v>
+      </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
+      <c r="L60" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>603</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" s="5">
+        <v>3</v>
+      </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
+      <c r="L61" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>700</v>
-      </c>
-      <c r="B62" t="s">
-        <v>41</v>
-      </c>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>701</v>
-      </c>
-      <c r="B63" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>1</v>
-      </c>
-      <c r="J63" s="3">
-        <v>1</v>
-      </c>
+      <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
-      </c>
-      <c r="C64" t="s">
-        <v>53</v>
-      </c>
-      <c r="D64">
-        <v>3</v>
-      </c>
-      <c r="E64" t="s">
-        <v>25</v>
-      </c>
-      <c r="F64">
-        <v>3</v>
-      </c>
-      <c r="H64">
-        <v>1</v>
-      </c>
-      <c r="J64" s="3">
-        <v>3</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C65" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F65">
-        <v>2</v>
-      </c>
-      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="H65" s="5">
         <v>1</v>
       </c>
       <c r="J65" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F66">
-        <v>2</v>
-      </c>
-      <c r="H66">
         <v>3</v>
       </c>
-      <c r="J66" s="3"/>
+      <c r="H66" s="5">
+        <v>1</v>
+      </c>
+      <c r="J66" s="3">
+        <v>3</v>
+      </c>
       <c r="K66" s="3"/>
-      <c r="L66" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C67" t="s">
         <v>52</v>
@@ -2014,133 +2054,144 @@
       <c r="F67">
         <v>2</v>
       </c>
-      <c r="H67">
-        <v>2</v>
-      </c>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3">
-        <v>2</v>
-      </c>
+      <c r="H67" s="5">
+        <v>1</v>
+      </c>
+      <c r="J67" s="3">
+        <v>2</v>
+      </c>
+      <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
+        <v>704</v>
+      </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="H68" s="5">
+        <v>3</v>
+      </c>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>705</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="H69" s="5">
+        <v>2</v>
+      </c>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3">
+        <v>2</v>
+      </c>
+      <c r="L69" s="3"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>707</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>64</v>
       </c>
-      <c r="D68">
-        <v>4</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70" t="s">
         <v>25</v>
       </c>
-      <c r="H68">
-        <v>2</v>
-      </c>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3">
-        <v>4</v>
-      </c>
-      <c r="L68" s="3"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="F70" s="4">
+        <v>2</v>
+      </c>
+      <c r="H70" s="5">
+        <v>2</v>
+      </c>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3">
+        <v>4</v>
+      </c>
+      <c r="L70" s="3"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>708</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>60</v>
       </c>
-      <c r="D69">
-        <v>4</v>
-      </c>
-      <c r="H69">
-        <v>3</v>
-      </c>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="H71" s="5">
+        <v>2</v>
+      </c>
       <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>800</v>
-      </c>
-      <c r="B72" t="s">
-        <v>78</v>
-      </c>
+      <c r="K71" s="3">
+        <v>4</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>801</v>
-      </c>
-      <c r="B73" t="s">
-        <v>80</v>
-      </c>
-      <c r="D73">
-        <v>5</v>
-      </c>
-      <c r="E73" t="s">
-        <v>16</v>
-      </c>
-      <c r="F73">
-        <v>5</v>
-      </c>
-      <c r="H73">
-        <v>1</v>
-      </c>
-      <c r="J73" s="3">
-        <v>5</v>
-      </c>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B74" t="s">
-        <v>79</v>
-      </c>
-      <c r="D74">
-        <v>10</v>
-      </c>
-      <c r="E74" t="s">
-        <v>16</v>
-      </c>
-      <c r="F74">
-        <v>10</v>
-      </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
-      <c r="J74" s="3">
-        <v>10</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D75">
         <v>5</v>
@@ -2151,7 +2202,7 @@
       <c r="F75">
         <v>5</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="5">
         <v>1</v>
       </c>
       <c r="J75" s="3">
@@ -2160,12 +2211,12 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D76">
         <v>10</v>
@@ -2173,7 +2224,10 @@
       <c r="E76" t="s">
         <v>16</v>
       </c>
-      <c r="H76">
+      <c r="F76">
+        <v>10</v>
+      </c>
+      <c r="H76" s="5">
         <v>1</v>
       </c>
       <c r="J76" s="3">
@@ -2182,47 +2236,98 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J77" s="3"/>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>803</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77">
+        <v>5</v>
+      </c>
+      <c r="E77" t="s">
+        <v>16</v>
+      </c>
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="H77" s="5">
+        <v>1</v>
+      </c>
+      <c r="J77" s="3">
+        <v>5</v>
+      </c>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>804</v>
+      </c>
+      <c r="B78" t="s">
+        <v>84</v>
+      </c>
       <c r="D78">
-        <f>SUM(D2:D77)</f>
-        <v>197</v>
-      </c>
-      <c r="F78">
-        <f>SUM(F2:F77)</f>
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="E78" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="5">
+        <v>1</v>
       </c>
       <c r="J78" s="3">
-        <f>SUM(J3:J77)</f>
-        <v>144</v>
-      </c>
-      <c r="K78" s="3">
-        <f>SUM(K3:K77)</f>
-        <v>22</v>
-      </c>
-      <c r="L78" s="3">
-        <f>SUM(L3:L77)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <f>SUM(D2:D79)</f>
+        <v>210</v>
+      </c>
+      <c r="F80">
+        <f>SUM(F2:F79)</f>
+        <v>135</v>
+      </c>
+      <c r="J80" s="3">
+        <f>SUM(J3:J79)</f>
+        <v>148</v>
+      </c>
+      <c r="K80" s="3">
+        <f>SUM(K3:K79)</f>
+        <v>39</v>
+      </c>
+      <c r="L80" s="3">
+        <f>SUM(L3:L79)</f>
+        <v>23</v>
+      </c>
+      <c r="N80">
+        <f>SUM(J80:M80)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
         <v>104</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F81" t="s">
         <v>100</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J81" t="s">
         <v>101</v>
       </c>
-      <c r="K79" t="s">
+      <c r="K81" t="s">
         <v>102</v>
       </c>
-      <c r="L79" t="s">
+      <c r="L81" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI updated, darkmode button
</commit_message>
<xml_diff>
--- a/ProjectFiles/Projektmanagement/Arbeitspakete.xlsx
+++ b/ProjectFiles/Projektmanagement/Arbeitspakete.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr showObjects="none" filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E4ACB3-10A5-4B1B-A833-F27631761B10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87FA6BD-DEAA-4E99-8B6E-F653B9E39326}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
   <si>
     <t>Nr</t>
   </si>
@@ -360,14 +360,34 @@
   </si>
   <si>
     <t>Rästel ausdenken/beschaffen</t>
+  </si>
+  <si>
+    <t>Statusbericht 16.03.</t>
+  </si>
+  <si>
+    <t>Statusbericht 22.03.</t>
+  </si>
+  <si>
+    <t>Tür und level completed</t>
+  </si>
+  <si>
+    <t>creditpage, controlpage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -428,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -437,6 +457,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -719,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,6 +803,18 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -836,6 +871,15 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
+      <c r="N4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4">
+        <v>40</v>
+      </c>
+      <c r="R4">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -864,6 +908,15 @@
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
+      <c r="N5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5">
+        <v>40</v>
+      </c>
+      <c r="R5">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -892,6 +945,15 @@
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
+      <c r="N6" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6">
+        <v>25</v>
+      </c>
+      <c r="R6">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -917,6 +979,15 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
+      <c r="N7" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7">
+        <v>25</v>
+      </c>
+      <c r="R7">
+        <v>130</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -942,23 +1013,90 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
+      <c r="N8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8">
+        <v>40</v>
+      </c>
+      <c r="R8">
+        <v>170</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J9" s="3"/>
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
+      <c r="N9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+      <c r="P9">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J10" s="3"/>
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
+      <c r="N10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -971,17 +1109,14 @@
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="N11" t="s">
-        <v>68</v>
-      </c>
-      <c r="O11" t="s">
-        <v>70</v>
-      </c>
-      <c r="P11" t="s">
-        <v>105</v>
-      </c>
-      <c r="R11" t="s">
-        <v>106</v>
+      <c r="N11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11">
+        <v>20</v>
+      </c>
+      <c r="P11">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1000,13 +1135,19 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="N13" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="O13">
-        <v>40</v>
-      </c>
-      <c r="R13">
-        <v>40</v>
+        <f>SUM(O4:O12)</f>
+        <v>220</v>
+      </c>
+      <c r="P13">
+        <f>SUM(P4:P12)</f>
+        <v>60</v>
+      </c>
+      <c r="Q13">
+        <f>SUM(O13:P13)</f>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1036,15 +1177,6 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="N14" t="s">
-        <v>71</v>
-      </c>
-      <c r="O14">
-        <v>40</v>
-      </c>
-      <c r="R14">
-        <v>80</v>
-      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1073,15 +1205,6 @@
       <c r="L15" s="3">
         <v>1</v>
       </c>
-      <c r="N15" t="s">
-        <v>72</v>
-      </c>
-      <c r="O15">
-        <v>25</v>
-      </c>
-      <c r="R15">
-        <v>105</v>
-      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1110,17 +1233,8 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="N16" t="s">
-        <v>73</v>
-      </c>
-      <c r="O16">
-        <v>25</v>
-      </c>
-      <c r="R16">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>204</v>
       </c>
@@ -1147,17 +1261,8 @@
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="N17" t="s">
-        <v>74</v>
-      </c>
-      <c r="O17">
-        <v>40</v>
-      </c>
-      <c r="R17">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>205</v>
       </c>
@@ -1165,6 +1270,9 @@
         <v>62</v>
       </c>
       <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="F18">
         <v>4</v>
       </c>
       <c r="H18" s="5">
@@ -1175,64 +1283,34 @@
       <c r="L18" s="3">
         <v>4</v>
       </c>
-      <c r="N18" t="s">
-        <v>75</v>
-      </c>
-      <c r="O18">
-        <v>20</v>
-      </c>
-      <c r="P18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19">
+    </row>
+    <row r="19" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
         <v>206</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D19">
+      <c r="H19" s="7">
+        <v>2</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8">
         <v>5</v>
       </c>
-      <c r="H19" s="5">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3">
-        <v>5</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="N19" t="s">
-        <v>76</v>
-      </c>
-      <c r="O19">
-        <v>20</v>
-      </c>
-      <c r="P19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="N20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O20">
-        <v>20</v>
-      </c>
-      <c r="P20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>300</v>
       </c>
@@ -1242,23 +1320,8 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="N22" t="s">
-        <v>82</v>
-      </c>
-      <c r="O22">
-        <f>SUM(O13:O21)</f>
-        <v>230</v>
-      </c>
-      <c r="P22">
-        <f>SUM(P13:P21)</f>
-        <v>60</v>
-      </c>
-      <c r="Q22">
-        <f>SUM(O22:P22)</f>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>301</v>
       </c>
@@ -1286,7 +1349,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>302</v>
       </c>
@@ -1303,7 +1366,7 @@
         <v>24</v>
       </c>
       <c r="F24">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H24" s="5">
         <v>1</v>
@@ -1314,7 +1377,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>303</v>
       </c>
@@ -1342,7 +1405,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>304</v>
       </c>
@@ -1367,7 +1430,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>305</v>
       </c>
@@ -1392,17 +1455,17 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>400</v>
       </c>
@@ -1413,32 +1476,27 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="31" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
         <v>401</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D31">
-        <v>5</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="5">
-        <v>2</v>
-      </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H31" s="7">
+        <v>2</v>
+      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -1558,6 +1616,9 @@
       <c r="E39" t="s">
         <v>26</v>
       </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
       <c r="H39" s="5">
         <v>1</v>
       </c>
@@ -1596,11 +1657,8 @@
       <c r="A41">
         <v>506</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
       </c>
       <c r="H41" s="5">
         <v>3</v>
@@ -1649,6 +1707,9 @@
       <c r="E43" t="s">
         <v>26</v>
       </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
       <c r="H43" s="5">
         <v>1</v>
       </c>
@@ -1671,8 +1732,8 @@
       <c r="E44" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="4">
-        <v>1</v>
+      <c r="F44">
+        <v>3</v>
       </c>
       <c r="H44" s="5">
         <v>2</v>
@@ -1696,6 +1757,9 @@
       <c r="E45" t="s">
         <v>25</v>
       </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
       <c r="H45" s="5">
         <v>2</v>
       </c>
@@ -1730,49 +1794,43 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="47" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
         <v>513</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D47">
-        <v>4</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="E47" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H47" s="5">
-        <v>2</v>
-      </c>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3">
-        <v>4</v>
-      </c>
-      <c r="L47" s="3"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="H47" s="7">
+        <v>2</v>
+      </c>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8">
+        <v>4</v>
+      </c>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
         <v>514</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="E48" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H48" s="5">
-        <v>2</v>
-      </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3">
-        <v>2</v>
-      </c>
-      <c r="L48" s="3"/>
+      <c r="H48" s="7">
+        <v>2</v>
+      </c>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8">
+        <v>2</v>
+      </c>
+      <c r="L48" s="8"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -1799,25 +1857,22 @@
       </c>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50">
+    <row r="50" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
         <v>516</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="E50" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H50" s="5">
+      <c r="H50" s="7">
         <v>3</v>
       </c>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3">
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1831,6 +1886,9 @@
       <c r="D51">
         <v>4</v>
       </c>
+      <c r="E51" t="s">
+        <v>93</v>
+      </c>
       <c r="F51">
         <v>4</v>
       </c>
@@ -1840,31 +1898,54 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row r="52" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
         <v>518</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D52">
-        <v>4</v>
-      </c>
-      <c r="H52" s="5">
-        <v>2</v>
-      </c>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3">
-        <v>4</v>
-      </c>
-      <c r="L52" s="3"/>
+      <c r="H52" s="7">
+        <v>2</v>
+      </c>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8">
+        <v>4</v>
+      </c>
+      <c r="L52" s="8"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J53" s="3"/>
+      <c r="A53">
+        <v>519</v>
+      </c>
+      <c r="B53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="H53" s="5">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3">
+        <v>2</v>
+      </c>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>520</v>
+      </c>
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -1898,41 +1979,35 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59">
+    <row r="59" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6">
         <v>601</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="H59" s="5">
+      <c r="H59" s="7">
         <v>3</v>
       </c>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6">
         <v>602</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="H60" s="5">
+      <c r="H60" s="7">
         <v>3</v>
       </c>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3">
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1940,7 +2015,7 @@
       <c r="A61">
         <v>603</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D61">
@@ -2132,8 +2207,8 @@
       <c r="E70" t="s">
         <v>25</v>
       </c>
-      <c r="F70" s="4">
-        <v>2</v>
+      <c r="F70">
+        <v>4</v>
       </c>
       <c r="H70" s="5">
         <v>2</v>
@@ -2152,6 +2227,12 @@
         <v>60</v>
       </c>
       <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>27</v>
+      </c>
+      <c r="F71">
         <v>4</v>
       </c>
       <c r="H71" s="5">
@@ -2274,6 +2355,9 @@
       <c r="E78" t="s">
         <v>16</v>
       </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
       <c r="H78" s="5">
         <v>1</v>
       </c>
@@ -2291,15 +2375,15 @@
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D80">
         <f>SUM(D2:D79)</f>
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="F80">
         <f>SUM(F2:F79)</f>
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="J80" s="3">
         <f>SUM(J3:J79)</f>
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="K80" s="3">
         <f>SUM(K3:K79)</f>
@@ -2307,11 +2391,11 @@
       </c>
       <c r="L80" s="3">
         <f>SUM(L3:L79)</f>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N80">
         <f>SUM(J80:M80)</f>
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="4:12" x14ac:dyDescent="0.3">
@@ -2333,5 +2417,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>